<commit_message>
subi facturas de ultimos gastos
</commit_message>
<xml_diff>
--- a/FINANZAS/CUADRO DE GASTOS 2020.xlsx
+++ b/FINANZAS/CUADRO DE GASTOS 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\fercho\empresas\modulo\repositorio\module\FINANZAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5372FA3D-46AB-47A8-B4A0-AEC1356B7DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9A6792-A942-4FBF-9D82-83941BD213BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{816B3DB9-02C2-4A5A-B155-018FAF001AFC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{816B3DB9-02C2-4A5A-B155-018FAF001AFC}"/>
   </bookViews>
   <sheets>
     <sheet name="AGOSTO 2020" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t xml:space="preserve">  CUADRO DE GASTOS </t>
   </si>
@@ -71,6 +71,21 @@
   </si>
   <si>
     <t>SEPTIEMBRE</t>
+  </si>
+  <si>
+    <t>arduino nano</t>
+  </si>
+  <si>
+    <t>conversor usbserial</t>
+  </si>
+  <si>
+    <t>baqulea 10x15</t>
+  </si>
+  <si>
+    <t>conversor ch340</t>
+  </si>
+  <si>
+    <t>conversor cp2102</t>
   </si>
 </sst>
 </file>
@@ -255,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -284,6 +299,7 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -896,7 +912,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,10 +989,18 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="17"/>
+      <c r="A5" s="14">
+        <v>44085</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1</v>
+      </c>
+      <c r="D5" s="17">
+        <v>13000</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -984,9 +1008,15 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="18">
+        <v>10000</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -994,19 +1024,33 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="18"/>
+      <c r="B7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="18">
+        <v>2600</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="14">
+        <v>44085</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="11">
+        <v>2</v>
+      </c>
+      <c r="D8" s="17">
+        <v>18000</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1014,9 +1058,15 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="18"/>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1</v>
+      </c>
+      <c r="D9" s="18">
+        <v>10000</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1128,14 +1178,14 @@
       </c>
       <c r="B20" s="20">
         <f>SUM(D5:D19)</f>
-        <v>0</v>
+        <v>53600</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="21">
         <f>(B20-F20)/2</f>
-        <v>0</v>
+        <v>26800</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>11</v>
@@ -1149,7 +1199,7 @@
       </c>
       <c r="H20" s="21">
         <f>(F20-B20)/2</f>
-        <v>0</v>
+        <v>-26800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadi facturas y actualice datos gastos
</commit_message>
<xml_diff>
--- a/FINANZAS/CUADRO DE GASTOS 2020.xlsx
+++ b/FINANZAS/CUADRO DE GASTOS 2020.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\PROJECTS\AEI PROJECT\AEI_IOT_V1.0\modulo\FINANZAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\fercho\empresas\modulo\repositorio\module\FINANZAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3E9828-158F-463B-B869-EEFFA6CBBA9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AGOSTO 2020" sheetId="1" r:id="rId1"/>
     <sheet name="SEPTIEMBRE 2020" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t xml:space="preserve">  CUADRO DE GASTOS </t>
   </si>
@@ -103,14 +104,17 @@
   </si>
   <si>
     <t>Arduino nano</t>
+  </si>
+  <si>
+    <t>sensor humedad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -285,7 +289,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -311,11 +315,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -638,11 +642,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,16 +936,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.140625" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -1138,20 +1143,36 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="18"/>
+      <c r="A10" s="14">
+        <v>44096</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="11">
+        <v>1</v>
+      </c>
+      <c r="D10" s="17">
+        <v>8000</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="18"/>
+      <c r="A11" s="14">
+        <v>44098</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="17">
+        <v>18000</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1243,14 +1264,14 @@
       </c>
       <c r="B20" s="20">
         <f>SUM(D5:D19)</f>
-        <v>53600</v>
+        <v>79600</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="21">
         <f>(B20-F20)/2</f>
-        <v>-39500</v>
+        <v>-26500</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>11</v>
@@ -1264,7 +1285,7 @@
       </c>
       <c r="H20" s="21">
         <f>(F20-B20)/2</f>
-        <v>39500</v>
+        <v>26500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>